<commit_message>
Calibrate electric v diesel rail
</commit_message>
<xml_diff>
--- a/InputData/trans/SYFAFE/Start Year Fleet Avg Fuel Economy.xlsx
+++ b/InputData/trans/SYFAFE/Start Year Fleet Avg Fuel Economy.xlsx
@@ -37,7 +37,7 @@
     <definedName name="ti_tbl_69" localSheetId="6">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="109">
   <si>
     <t>Sources:</t>
   </si>
@@ -7582,10 +7582,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BT57"/>
+  <dimension ref="A1:BT58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection sqref="A1:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -8874,211 +8874,211 @@
         <v>42</v>
       </c>
       <c r="C8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="D8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="E8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="F8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="G8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="H8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="I8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="J8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="K8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="L8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="M8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="N8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="O8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="P8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="Q8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="R8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="S8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="T8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="U8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="V8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="W8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="X8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="Y8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="Z8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="AA8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="AB8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="AC8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="AD8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="AE8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="AF8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="AG8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="AH8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="AI8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="AJ8" s="21">
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="AK8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="AL8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="AM8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="AN8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="AO8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="AP8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="AQ8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="AR8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="AS8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="AT8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="AU8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="AV8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="AW8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="AX8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="AY8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="AZ8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BA8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BB8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BC8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BD8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BE8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BF8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BG8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BH8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BI8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BJ8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BK8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BL8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BM8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BN8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BO8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BP8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BQ8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BR8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BS8" s="23">
-        <v>2.1558990043642106E-3</v>
+        <v>1.9391498614175121E-2</v>
       </c>
       <c r="BT8" s="18"/>
     </row>
@@ -9090,211 +9090,211 @@
         <v>42</v>
       </c>
       <c r="C9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="D9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="E9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="F9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="G9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="H9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="I9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="J9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="K9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="L9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="M9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="N9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="O9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="P9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="Q9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="R9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="S9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="T9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="U9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="V9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="W9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="X9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="Y9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="Z9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="AA9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="AB9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="AC9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="AD9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="AE9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="AF9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="AG9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="AH9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="AI9" s="18">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="AJ9" s="16">
-        <v>1.0487527988911177E-2</v>
+        <v>1.0424816773970053E-2</v>
       </c>
       <c r="AK9" s="23">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="AL9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="AM9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="AN9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="AO9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="AP9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="AQ9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="AR9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="AS9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="AT9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="AU9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="AV9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="AW9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="AX9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="AY9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="AZ9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BA9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BB9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BC9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BD9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BE9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BF9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BG9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BH9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BI9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BJ9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BK9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BL9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BM9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BN9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BO9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BP9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BQ9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BR9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BS9" s="22">
-        <v>1.0487527988911182E-2</v>
+        <v>1.0424816773970049E-2</v>
       </c>
       <c r="BT9" s="18"/>
     </row>
@@ -9306,425 +9306,427 @@
         <v>43</v>
       </c>
       <c r="C10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="D10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="E10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="F10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="G10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="H10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="I10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="J10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="K10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="L10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="M10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="N10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="O10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="P10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="Q10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="R10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="S10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="T10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="U10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="V10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="W10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="X10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="Y10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="Z10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="AA10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="AB10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="AC10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="AD10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="AE10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="AF10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="AG10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="AH10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="AI10" s="18">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="AJ10" s="16">
-        <v>7.0214683806076091E-3</v>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="AK10" s="23">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="AL10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="AM10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="AN10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="AO10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="AP10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="AQ10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="AR10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="AS10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="AT10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="AU10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="AV10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="AW10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="AX10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="AY10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="AZ10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BA10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BB10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BC10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BD10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BE10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BF10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BG10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BH10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BI10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BJ10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BK10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BL10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BM10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BN10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BO10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BP10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BQ10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BR10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BS10" s="22">
-        <v>7.0214683806076135E-3</v>
+        <v>1.3495815062532838E-2</v>
       </c>
       <c r="BT10" s="18"/>
     </row>
     <row r="11" spans="1:72">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="14"/>
+        <v>43</v>
+      </c>
+      <c r="C11" s="18">
+        <v>3.7455550122320706E-3</v>
+      </c>
       <c r="D11" s="18">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="E11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="F11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="G11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="H11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="I11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="J11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="K11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="L11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="M11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="N11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="O11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="P11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="Q11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="R11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="S11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="T11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="U11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="V11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="W11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="X11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="Y11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="Z11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="AA11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="AB11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="AC11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="AD11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="AE11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="AF11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="AG11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="AH11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="AI11" s="18">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="AJ11" s="16">
-        <v>1.9362141353943097E-4</v>
+        <v>3.7455550122320706E-3</v>
       </c>
       <c r="AK11" s="23">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="AL11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="AM11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="AN11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="AO11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="AP11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="AQ11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="AR11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="AS11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="AT11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="AU11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="AV11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="AW11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="AX11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="AY11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="AZ11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BA11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BB11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BC11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BD11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BE11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BF11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BG11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BH11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BI11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BJ11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BK11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BL11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BM11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BN11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BO11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BP11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BQ11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BR11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BS11" s="22">
-        <v>1.9362141353943107E-4</v>
+        <v>3.7455550122320676E-3</v>
       </c>
       <c r="BT11" s="18"/>
     </row>
@@ -9733,407 +9735,453 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="18">
-        <v>3.3209939763395591E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="E12" s="18">
-        <v>3.3814550029391821E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="F12" s="18">
-        <v>3.441916029538819E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="G12" s="18">
-        <v>3.5023770561384421E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="H12" s="18">
-        <v>3.5628380827380651E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="I12" s="18">
-        <v>3.6232991093377021E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="J12" s="18">
-        <v>3.6837601359373251E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="K12" s="18">
-        <v>3.7442211625369481E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="L12" s="18">
-        <v>3.8046821891365851E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="M12" s="18">
-        <v>3.8651432157362081E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="N12" s="18">
-        <v>3.925604242335845E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="O12" s="18">
-        <v>3.9860652689354681E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="P12" s="18">
-        <v>4.0465262955350911E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="Q12" s="18">
-        <v>4.1069873221347281E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="R12" s="18">
-        <v>4.1674483487343511E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="S12" s="18">
-        <v>4.2279093753339742E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="T12" s="18">
-        <v>4.2883704019336111E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="U12" s="18">
-        <v>4.3488314285332341E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="V12" s="18">
-        <v>4.409292455132871E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="W12" s="18">
-        <v>4.4697534817324941E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="X12" s="18">
-        <v>4.5302145083321171E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="Y12" s="18">
-        <v>4.5906755349317541E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="Z12" s="18">
-        <v>4.6511365615313771E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="AA12" s="18">
-        <v>4.7115975881310002E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="AB12" s="18">
-        <v>4.7720586147306371E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="AC12" s="18">
-        <v>4.8325196413302601E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="AD12" s="18">
-        <v>4.8929806679298971E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="AE12" s="18">
-        <v>4.9534416945295201E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="AF12" s="18">
-        <v>5.0139027211291431E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="AG12" s="18">
-        <v>5.0743637477287801E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="AH12" s="18">
-        <v>5.1348247743284031E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="AI12" s="18">
-        <v>5.1952858009280262E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="AJ12" s="16">
-        <v>5.2557468275276631E-3</v>
+        <v>1.9362141353943097E-4</v>
       </c>
       <c r="AK12" s="23">
-        <v>5.2992115229405527E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="AL12" s="22">
-        <v>5.2992115229405527E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="AM12" s="22">
-        <v>5.3934315680825738E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="AN12" s="22">
-        <v>5.4328972597188054E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="AO12" s="22">
-        <v>5.4639690719479918E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="AP12" s="22">
-        <v>5.5418412974535475E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="AQ12" s="22">
-        <v>5.6194390279456462E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="AR12" s="22">
-        <v>5.6977290697036269E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="AS12" s="22">
-        <v>5.7753683101031145E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="AT12" s="22">
-        <v>5.8065339689778806E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="AU12" s="22">
-        <v>5.9168077326028174E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="AV12" s="22">
-        <v>6.0262008784596468E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="AW12" s="22">
-        <v>6.1333911053254144E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="AX12" s="22">
-        <v>6.23926005928913E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="AY12" s="22">
-        <v>6.2631866999947458E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="AZ12" s="22">
-        <v>6.3166177586814537E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BA12" s="22">
-        <v>6.3698985412702644E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BB12" s="22">
-        <v>6.4221337603906021E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BC12" s="22">
-        <v>6.4770178768907465E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BD12" s="22">
-        <v>6.5040881848864238E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BE12" s="22">
-        <v>6.5657441588667436E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BF12" s="22">
-        <v>6.6279838592649453E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BG12" s="22">
-        <v>6.6926091644649984E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BH12" s="22">
-        <v>6.7592235851418906E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BI12" s="22">
-        <v>6.8261740810624423E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BJ12" s="22">
-        <v>6.8617594497521082E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BK12" s="22">
-        <v>6.9004780853928341E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BL12" s="22">
-        <v>6.9410482983891979E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BM12" s="22">
-        <v>6.9822916342727305E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BN12" s="22">
-        <v>7.0276191171519658E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BO12" s="22">
-        <v>7.0718499244147234E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BP12" s="22">
-        <v>7.1189794928731096E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BQ12" s="22">
-        <v>7.1700377368293525E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BR12" s="22">
-        <v>7.221347583681044E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BS12" s="22">
-        <v>7.2762043320700196E-3</v>
+        <v>1.9362141353943107E-4</v>
       </c>
       <c r="BT12" s="18"/>
     </row>
     <row r="13" spans="1:72">
       <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="18">
+        <v>3.3209939763395591E-3</v>
+      </c>
+      <c r="E13" s="18">
+        <v>3.3814550029391821E-3</v>
+      </c>
+      <c r="F13" s="18">
+        <v>3.441916029538819E-3</v>
+      </c>
+      <c r="G13" s="18">
+        <v>3.5023770561384421E-3</v>
+      </c>
+      <c r="H13" s="18">
+        <v>3.5628380827380651E-3</v>
+      </c>
+      <c r="I13" s="18">
+        <v>3.6232991093377021E-3</v>
+      </c>
+      <c r="J13" s="18">
+        <v>3.6837601359373251E-3</v>
+      </c>
+      <c r="K13" s="18">
+        <v>3.7442211625369481E-3</v>
+      </c>
+      <c r="L13" s="18">
+        <v>3.8046821891365851E-3</v>
+      </c>
+      <c r="M13" s="18">
+        <v>3.8651432157362081E-3</v>
+      </c>
+      <c r="N13" s="18">
+        <v>3.925604242335845E-3</v>
+      </c>
+      <c r="O13" s="18">
+        <v>3.9860652689354681E-3</v>
+      </c>
+      <c r="P13" s="18">
+        <v>4.0465262955350911E-3</v>
+      </c>
+      <c r="Q13" s="18">
+        <v>4.1069873221347281E-3</v>
+      </c>
+      <c r="R13" s="18">
+        <v>4.1674483487343511E-3</v>
+      </c>
+      <c r="S13" s="18">
+        <v>4.2279093753339742E-3</v>
+      </c>
+      <c r="T13" s="18">
+        <v>4.2883704019336111E-3</v>
+      </c>
+      <c r="U13" s="18">
+        <v>4.3488314285332341E-3</v>
+      </c>
+      <c r="V13" s="18">
+        <v>4.409292455132871E-3</v>
+      </c>
+      <c r="W13" s="18">
+        <v>4.4697534817324941E-3</v>
+      </c>
+      <c r="X13" s="18">
+        <v>4.5302145083321171E-3</v>
+      </c>
+      <c r="Y13" s="18">
+        <v>4.5906755349317541E-3</v>
+      </c>
+      <c r="Z13" s="18">
+        <v>4.6511365615313771E-3</v>
+      </c>
+      <c r="AA13" s="18">
+        <v>4.7115975881310002E-3</v>
+      </c>
+      <c r="AB13" s="18">
+        <v>4.7720586147306371E-3</v>
+      </c>
+      <c r="AC13" s="18">
+        <v>4.8325196413302601E-3</v>
+      </c>
+      <c r="AD13" s="18">
+        <v>4.8929806679298971E-3</v>
+      </c>
+      <c r="AE13" s="18">
+        <v>4.9534416945295201E-3</v>
+      </c>
+      <c r="AF13" s="18">
+        <v>5.0139027211291431E-3</v>
+      </c>
+      <c r="AG13" s="18">
+        <v>5.0743637477287801E-3</v>
+      </c>
+      <c r="AH13" s="18">
+        <v>5.1348247743284031E-3</v>
+      </c>
+      <c r="AI13" s="18">
+        <v>5.1952858009280262E-3</v>
+      </c>
+      <c r="AJ13" s="16">
+        <v>5.2557468275276631E-3</v>
+      </c>
+      <c r="AK13" s="23">
+        <v>5.2992115229405527E-3</v>
+      </c>
+      <c r="AL13" s="22">
+        <v>5.2992115229405527E-3</v>
+      </c>
+      <c r="AM13" s="22">
+        <v>5.3934315680825738E-3</v>
+      </c>
+      <c r="AN13" s="22">
+        <v>5.4328972597188054E-3</v>
+      </c>
+      <c r="AO13" s="22">
+        <v>5.4639690719479918E-3</v>
+      </c>
+      <c r="AP13" s="22">
+        <v>5.5418412974535475E-3</v>
+      </c>
+      <c r="AQ13" s="22">
+        <v>5.6194390279456462E-3</v>
+      </c>
+      <c r="AR13" s="22">
+        <v>5.6977290697036269E-3</v>
+      </c>
+      <c r="AS13" s="22">
+        <v>5.7753683101031145E-3</v>
+      </c>
+      <c r="AT13" s="22">
+        <v>5.8065339689778806E-3</v>
+      </c>
+      <c r="AU13" s="22">
+        <v>5.9168077326028174E-3</v>
+      </c>
+      <c r="AV13" s="22">
+        <v>6.0262008784596468E-3</v>
+      </c>
+      <c r="AW13" s="22">
+        <v>6.1333911053254144E-3</v>
+      </c>
+      <c r="AX13" s="22">
+        <v>6.23926005928913E-3</v>
+      </c>
+      <c r="AY13" s="22">
+        <v>6.2631866999947458E-3</v>
+      </c>
+      <c r="AZ13" s="22">
+        <v>6.3166177586814537E-3</v>
+      </c>
+      <c r="BA13" s="22">
+        <v>6.3698985412702644E-3</v>
+      </c>
+      <c r="BB13" s="22">
+        <v>6.4221337603906021E-3</v>
+      </c>
+      <c r="BC13" s="22">
+        <v>6.4770178768907465E-3</v>
+      </c>
+      <c r="BD13" s="22">
+        <v>6.5040881848864238E-3</v>
+      </c>
+      <c r="BE13" s="22">
+        <v>6.5657441588667436E-3</v>
+      </c>
+      <c r="BF13" s="22">
+        <v>6.6279838592649453E-3</v>
+      </c>
+      <c r="BG13" s="22">
+        <v>6.6926091644649984E-3</v>
+      </c>
+      <c r="BH13" s="22">
+        <v>6.7592235851418906E-3</v>
+      </c>
+      <c r="BI13" s="22">
+        <v>6.8261740810624423E-3</v>
+      </c>
+      <c r="BJ13" s="22">
+        <v>6.8617594497521082E-3</v>
+      </c>
+      <c r="BK13" s="22">
+        <v>6.9004780853928341E-3</v>
+      </c>
+      <c r="BL13" s="22">
+        <v>6.9410482983891979E-3</v>
+      </c>
+      <c r="BM13" s="22">
+        <v>6.9822916342727305E-3</v>
+      </c>
+      <c r="BN13" s="22">
+        <v>7.0276191171519658E-3</v>
+      </c>
+      <c r="BO13" s="22">
+        <v>7.0718499244147234E-3</v>
+      </c>
+      <c r="BP13" s="22">
+        <v>7.1189794928731096E-3</v>
+      </c>
+      <c r="BQ13" s="22">
+        <v>7.1700377368293525E-3</v>
+      </c>
+      <c r="BR13" s="22">
+        <v>7.221347583681044E-3</v>
+      </c>
+      <c r="BS13" s="22">
+        <v>7.2762043320700196E-3</v>
+      </c>
+      <c r="BT13" s="18"/>
+    </row>
+    <row r="14" spans="1:72">
+      <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="14"/>
-      <c r="V13" s="14"/>
-      <c r="W13" s="14"/>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="14"/>
-      <c r="AA13" s="18">
-        <v>1.5431879298095448E-3</v>
-      </c>
-      <c r="AB13" s="18">
-        <v>1.5431879298095448E-3</v>
-      </c>
-      <c r="AC13" s="18">
-        <v>1.5431879298095448E-3</v>
-      </c>
-      <c r="AD13" s="18">
-        <v>1.5431879298095448E-3</v>
-      </c>
-      <c r="AE13" s="18">
-        <v>1.5431879298095448E-3</v>
-      </c>
-      <c r="AF13" s="18">
-        <v>1.5431879298095448E-3</v>
-      </c>
-      <c r="AG13" s="18">
-        <v>1.5431879298095448E-3</v>
-      </c>
-      <c r="AH13" s="18">
-        <v>1.5431879298095448E-3</v>
-      </c>
-      <c r="AI13" s="18">
-        <v>1.5431879298095448E-3</v>
-      </c>
-      <c r="AJ13" s="16">
-        <v>1.5431879298095448E-3</v>
-      </c>
-      <c r="AK13" s="23">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="AL13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="AM13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="AN13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="AO13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="AP13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="AQ13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="AR13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="AS13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="AT13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="AU13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="AV13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="AW13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="AX13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="AY13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="AZ13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BA13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BB13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BC13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BD13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BE13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BF13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BG13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BH13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BI13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BJ13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BK13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BL13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BM13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BN13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BO13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BP13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BQ13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BR13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BS13" s="22">
-        <v>1.5431879298095457E-3</v>
-      </c>
-      <c r="BT13" s="18"/>
-    </row>
-    <row r="14" spans="1:72" s="8" customFormat="1">
-      <c r="A14" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="19"/>
-      <c r="S14" s="19"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
       <c r="T14" s="14"/>
       <c r="U14" s="14"/>
       <c r="V14" s="14"/>
@@ -10142,224 +10190,372 @@
       <c r="Y14" s="14"/>
       <c r="Z14" s="14"/>
       <c r="AA14" s="18">
+        <v>1.5431879298095448E-3</v>
+      </c>
+      <c r="AB14" s="18">
+        <v>1.5431879298095448E-3</v>
+      </c>
+      <c r="AC14" s="18">
+        <v>1.5431879298095448E-3</v>
+      </c>
+      <c r="AD14" s="18">
+        <v>1.5431879298095448E-3</v>
+      </c>
+      <c r="AE14" s="18">
+        <v>1.5431879298095448E-3</v>
+      </c>
+      <c r="AF14" s="18">
+        <v>1.5431879298095448E-3</v>
+      </c>
+      <c r="AG14" s="18">
+        <v>1.5431879298095448E-3</v>
+      </c>
+      <c r="AH14" s="18">
+        <v>1.5431879298095448E-3</v>
+      </c>
+      <c r="AI14" s="18">
+        <v>1.5431879298095448E-3</v>
+      </c>
+      <c r="AJ14" s="16">
+        <v>1.5431879298095448E-3</v>
+      </c>
+      <c r="AK14" s="23">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="AL14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="AM14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="AN14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="AO14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="AP14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="AQ14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="AR14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="AS14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="AT14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="AU14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="AV14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="AW14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="AX14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="AY14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="AZ14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BA14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BB14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BC14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BD14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BE14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BF14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BG14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BH14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BI14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BJ14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BK14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BL14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BM14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BN14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BO14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BP14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BQ14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BR14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BS14" s="22">
+        <v>1.5431879298095457E-3</v>
+      </c>
+      <c r="BT14" s="18"/>
+    </row>
+    <row r="15" spans="1:72" s="8" customFormat="1">
+      <c r="A15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
+      <c r="Y15" s="14"/>
+      <c r="Z15" s="14"/>
+      <c r="AA15" s="18">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AB14" s="18">
+      <c r="AB15" s="18">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AC14" s="18">
+      <c r="AC15" s="18">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AD14" s="18">
+      <c r="AD15" s="18">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AE14" s="18">
+      <c r="AE15" s="18">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AF14" s="18">
+      <c r="AF15" s="18">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AG14" s="18">
+      <c r="AG15" s="18">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AH14" s="18">
+      <c r="AH15" s="18">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AI14" s="18">
+      <c r="AI15" s="18">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AJ14" s="16">
+      <c r="AJ15" s="16">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AK14" s="23">
+      <c r="AK15" s="23">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AL14" s="22">
+      <c r="AL15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AM14" s="22">
+      <c r="AM15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AN14" s="22">
+      <c r="AN15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AO14" s="22">
+      <c r="AO15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AP14" s="22">
+      <c r="AP15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AQ14" s="22">
+      <c r="AQ15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AR14" s="22">
+      <c r="AR15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AS14" s="22">
+      <c r="AS15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AT14" s="22">
+      <c r="AT15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AU14" s="22">
+      <c r="AU15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AV14" s="22">
+      <c r="AV15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AW14" s="22">
+      <c r="AW15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AX14" s="22">
+      <c r="AX15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AY14" s="22">
+      <c r="AY15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="AZ14" s="22">
+      <c r="AZ15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="BA14" s="22">
+      <c r="BA15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="BB14" s="22">
+      <c r="BB15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="BC14" s="22">
+      <c r="BC15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="BD14" s="22">
+      <c r="BD15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="BE14" s="22">
+      <c r="BE15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="BF14" s="22">
+      <c r="BF15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="BG14" s="22">
+      <c r="BG15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="BH14" s="22">
+      <c r="BH15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="BI14" s="22">
+      <c r="BI15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="BJ14" s="22">
+      <c r="BJ15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="BK14" s="22">
+      <c r="BK15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="BL14" s="22">
+      <c r="BL15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="BM14" s="22">
+      <c r="BM15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="BN14" s="22">
+      <c r="BN15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="BO14" s="22">
+      <c r="BO15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="BP14" s="22">
+      <c r="BP15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="BQ14" s="22">
+      <c r="BQ15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="BR14" s="22">
+      <c r="BR15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
-      <c r="BS14" s="22">
+      <c r="BS15" s="22">
         <v>1.1883392852619099E-3</v>
       </c>
     </row>
-    <row r="47" spans="3:8">
-      <c r="C47" t="s">
+    <row r="48" spans="3:8">
+      <c r="C48" t="s">
         <v>64</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>101</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E48" t="s">
         <v>102</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F48" t="s">
         <v>103</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G48" t="s">
         <v>104</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H48" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="48" spans="3:8">
-      <c r="C48">
-        <v>2021</v>
-      </c>
-      <c r="D48">
-        <v>20.709724091851811</v>
-      </c>
-      <c r="E48">
-        <v>1560.8681637371849</v>
-      </c>
-      <c r="F48">
-        <v>411.91631433310613</v>
-      </c>
-      <c r="G48">
-        <v>2.4276775772258579E-3</v>
-      </c>
-      <c r="H48">
-        <v>1.5084926598642038E-3</v>
       </c>
     </row>
     <row r="49" spans="3:48">
       <c r="C49">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="D49">
-        <v>18.004733712284658</v>
+        <v>20.709724091851811</v>
       </c>
       <c r="E49">
-        <v>1795.3694584606365</v>
+        <v>1560.8681637371849</v>
       </c>
       <c r="F49">
-        <v>473.80168766120875</v>
+        <v>411.91631433310613</v>
       </c>
       <c r="G49">
-        <v>2.1105876699937984E-3</v>
+        <v>2.4276775772258579E-3</v>
       </c>
       <c r="H49">
-        <v>1.3114616364433857E-3</v>
+        <v>1.5084926598642038E-3</v>
       </c>
     </row>
     <row r="50" spans="3:48">
       <c r="C50">
-        <v>2012</v>
+        <v>2016</v>
       </c>
       <c r="D50">
-        <v>17.211393460387786</v>
+        <v>18.004733712284658</v>
       </c>
       <c r="E50">
-        <v>1878.1250390416772</v>
+        <v>1795.3694584606365</v>
       </c>
       <c r="F50">
-        <v>495.64105535118767</v>
+        <v>473.80168766120875</v>
       </c>
       <c r="G50">
-        <v>2.0175891185839068E-3</v>
+        <v>2.1105876699937984E-3</v>
       </c>
       <c r="H50">
-        <v>1.2536748720493537E-3</v>
+        <v>1.3114616364433857E-3</v>
       </c>
     </row>
     <row r="51" spans="3:48">
       <c r="C51">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D51">
         <v>17.211393460387786</v>
@@ -10379,338 +10575,358 @@
     </row>
     <row r="52" spans="3:48">
       <c r="C52">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="D52">
-        <v>16.96226746103957</v>
+        <v>17.211393460387786</v>
       </c>
       <c r="E52">
-        <v>1905.7091918282579</v>
+        <v>1878.1250390416772</v>
       </c>
       <c r="F52">
-        <v>502.92056992764282</v>
+        <v>495.64105535118767</v>
       </c>
       <c r="G52">
-        <v>1.9883855618470208E-3</v>
+        <v>2.0175891185839068E-3</v>
       </c>
       <c r="H52">
-        <v>1.2355285780798469E-3</v>
+        <v>1.2536748720493537E-3</v>
       </c>
     </row>
     <row r="53" spans="3:48">
       <c r="C53">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="D53">
-        <v>16.601821590736861</v>
+        <v>16.96226746103957</v>
       </c>
       <c r="E53">
-        <v>1947.0844713081717</v>
+        <v>1905.7091918282579</v>
       </c>
       <c r="F53">
-        <v>513.83959116455617</v>
+        <v>502.92056992764282</v>
       </c>
       <c r="G53">
-        <v>1.9461326398256297E-3</v>
+        <v>1.9883855618470208E-3</v>
       </c>
       <c r="H53">
-        <v>1.2092737642919642E-3</v>
+        <v>1.2355285780798469E-3</v>
       </c>
     </row>
     <row r="54" spans="3:48">
       <c r="C54">
+        <v>2009</v>
+      </c>
+      <c r="D54">
+        <v>16.601821590736861</v>
+      </c>
+      <c r="E54">
+        <v>1947.0844713081717</v>
+      </c>
+      <c r="F54">
+        <v>513.83959116455617</v>
+      </c>
+      <c r="G54">
+        <v>1.9461326398256297E-3</v>
+      </c>
+      <c r="H54">
+        <v>1.2092737642919642E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="3:48">
+      <c r="C55">
         <v>2006</v>
       </c>
-      <c r="D54">
+      <c r="D55">
         <v>15.301305075439725</v>
       </c>
-      <c r="E54">
+      <c r="E55">
         <v>2112.5746369594244</v>
       </c>
-      <c r="F54">
+      <c r="F55">
         <v>557.51278578608299</v>
       </c>
-      <c r="G54">
+      <c r="G55">
         <v>1.7936808365569912E-3</v>
       </c>
-      <c r="H54">
+      <c r="H55">
         <v>1.1145443700877325E-3</v>
       </c>
     </row>
-    <row r="56" spans="3:48">
-      <c r="D56">
+    <row r="57" spans="3:48">
+      <c r="D57">
         <v>2006</v>
       </c>
-      <c r="E56">
+      <c r="E57">
         <v>2007</v>
       </c>
-      <c r="F56">
+      <c r="F57">
         <v>2008</v>
       </c>
-      <c r="G56">
+      <c r="G57">
         <v>2009</v>
       </c>
-      <c r="H56">
+      <c r="H57">
         <v>2010</v>
       </c>
-      <c r="I56">
+      <c r="I57">
         <v>2011</v>
       </c>
-      <c r="J56">
+      <c r="J57">
         <v>2012</v>
       </c>
-      <c r="K56">
+      <c r="K57">
         <v>2013</v>
       </c>
-      <c r="L56">
+      <c r="L57">
         <v>2014</v>
       </c>
-      <c r="M56">
+      <c r="M57">
         <v>2015</v>
       </c>
-      <c r="N56">
+      <c r="N57">
         <v>2016</v>
       </c>
-      <c r="O56">
+      <c r="O57">
         <v>2017</v>
       </c>
-      <c r="P56">
+      <c r="P57">
         <v>2018</v>
       </c>
-      <c r="Q56">
+      <c r="Q57">
         <v>2019</v>
       </c>
-      <c r="R56">
+      <c r="R57">
         <v>2020</v>
       </c>
-      <c r="S56">
+      <c r="S57">
         <v>2021</v>
       </c>
-      <c r="T56">
+      <c r="T57">
         <v>2022</v>
       </c>
-      <c r="U56">
+      <c r="U57">
         <v>2023</v>
       </c>
-      <c r="V56">
+      <c r="V57">
         <v>2024</v>
       </c>
-      <c r="W56">
+      <c r="W57">
         <v>2025</v>
       </c>
-      <c r="X56">
+      <c r="X57">
         <v>2026</v>
       </c>
-      <c r="Y56">
+      <c r="Y57">
         <v>2027</v>
       </c>
-      <c r="Z56">
+      <c r="Z57">
         <v>2028</v>
       </c>
-      <c r="AA56">
+      <c r="AA57">
         <v>2029</v>
       </c>
-      <c r="AB56">
+      <c r="AB57">
         <v>2030</v>
       </c>
-      <c r="AC56">
+      <c r="AC57">
         <v>2031</v>
       </c>
-      <c r="AD56">
+      <c r="AD57">
         <v>2032</v>
       </c>
-      <c r="AE56">
+      <c r="AE57">
         <v>2033</v>
       </c>
-      <c r="AF56">
+      <c r="AF57">
         <v>2034</v>
       </c>
-      <c r="AG56">
+      <c r="AG57">
         <v>2035</v>
       </c>
-      <c r="AH56">
+      <c r="AH57">
         <v>2036</v>
       </c>
-      <c r="AI56">
+      <c r="AI57">
         <v>2037</v>
       </c>
-      <c r="AJ56">
+      <c r="AJ57">
         <v>2038</v>
       </c>
-      <c r="AK56">
+      <c r="AK57">
         <v>2039</v>
       </c>
-      <c r="AL56">
+      <c r="AL57">
         <v>2040</v>
       </c>
-      <c r="AM56">
+      <c r="AM57">
         <v>2041</v>
       </c>
-      <c r="AN56">
+      <c r="AN57">
         <v>2042</v>
       </c>
-      <c r="AO56">
+      <c r="AO57">
         <v>2043</v>
       </c>
-      <c r="AP56">
+      <c r="AP57">
         <v>2044</v>
       </c>
-      <c r="AQ56">
+      <c r="AQ57">
         <v>2045</v>
       </c>
-      <c r="AR56">
+      <c r="AR57">
         <v>2046</v>
       </c>
-      <c r="AS56">
+      <c r="AS57">
         <v>2047</v>
       </c>
-      <c r="AT56">
+      <c r="AT57">
         <v>2048</v>
       </c>
-      <c r="AU56">
+      <c r="AU57">
         <v>2049</v>
       </c>
-      <c r="AV56">
+      <c r="AV57">
         <v>2050</v>
       </c>
     </row>
-    <row r="57" spans="3:48">
-      <c r="C57" t="s">
+    <row r="58" spans="3:48">
+      <c r="C58" t="s">
         <v>106</v>
       </c>
-      <c r="D57">
+      <c r="D58">
         <v>6.5405985853042581E-4</v>
       </c>
-      <c r="E57">
+      <c r="E58">
         <v>6.7259020923837731E-4</v>
       </c>
-      <c r="F57">
+      <c r="F58">
         <v>6.9112055994632882E-4</v>
       </c>
-      <c r="G57">
+      <c r="G58">
         <v>7.0965091065427772E-4</v>
       </c>
-      <c r="H57">
+      <c r="H58">
         <v>7.2505830066289041E-4</v>
       </c>
-      <c r="I57">
+      <c r="I58">
         <v>7.3570728224234326E-4</v>
       </c>
-      <c r="J57">
+      <c r="J58">
         <v>7.3570728224234272E-4</v>
       </c>
-      <c r="K57">
+      <c r="K58">
         <v>7.4418518674728568E-4</v>
       </c>
-      <c r="L57">
+      <c r="L58">
         <v>7.5266309125222516E-4</v>
       </c>
-      <c r="M57">
+      <c r="M58">
         <v>7.6114099575716465E-4</v>
       </c>
-      <c r="N57">
+      <c r="N58">
         <v>7.6961890026210566E-4</v>
       </c>
-      <c r="O57">
+      <c r="O58">
         <v>7.9274406006073217E-4</v>
       </c>
-      <c r="P57">
+      <c r="P58">
         <v>8.1586921985937061E-4</v>
       </c>
-      <c r="Q57">
+      <c r="Q58">
         <v>8.3899437965800211E-4</v>
       </c>
-      <c r="R57">
+      <c r="R58">
         <v>8.6211953945663361E-4</v>
       </c>
-      <c r="S57">
+      <c r="S58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="T57">
+      <c r="T58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="U57">
+      <c r="U58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="V57">
+      <c r="V58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="W57">
+      <c r="W58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="X57">
+      <c r="X58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="Y57">
+      <c r="Y58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="Z57">
+      <c r="Z58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AA57">
+      <c r="AA58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AB57">
+      <c r="AB58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AC57">
+      <c r="AC58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AD57">
+      <c r="AD58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AE57">
+      <c r="AE58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AF57">
+      <c r="AF58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AG57">
+      <c r="AG58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AH57">
+      <c r="AH58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AI57">
+      <c r="AI58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AJ57">
+      <c r="AJ58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AK57">
+      <c r="AK58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AL57">
+      <c r="AL58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AM57">
+      <c r="AM58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AN57">
+      <c r="AN58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AO57">
+      <c r="AO58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AP57">
+      <c r="AP58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AQ57">
+      <c r="AQ58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AR57">
+      <c r="AR58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AS57">
+      <c r="AS58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AT57">
+      <c r="AT58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AU57">
+      <c r="AU58">
         <v>8.8524469925526836E-4</v>
       </c>
-      <c r="AV57">
+      <c r="AV58">
         <v>8.8524469925526836E-4</v>
       </c>
     </row>
@@ -11343,7 +11559,7 @@
       </c>
       <c r="B5" s="18">
         <f>AVERAGE('BHNVFEAL data'!C8:AJ8)*'Calibration Adjustments'!E22</f>
-        <v>2.1558990043642106E-3</v>
+        <v>1.939149861417511E-2</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -11353,7 +11569,7 @@
       </c>
       <c r="E5" s="18">
         <f>AVERAGE('BHNVFEAL data'!C9:AJ9)*'Calibration Adjustments'!E22</f>
-        <v>1.0487527988911173E-2</v>
+        <v>1.0424816773970056E-2</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -11379,7 +11595,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="18">
-        <f>AVERAGE('BHNVFEAL data'!D11:AJ11)*'Calibration Adjustments'!E23</f>
+        <f>AVERAGE('BHNVFEAL data'!D12:AJ12)*'Calibration Adjustments'!E23</f>
         <v>1.9362141353943094E-4</v>
       </c>
       <c r="F6">
@@ -11405,7 +11621,7 @@
         <v>1.5431879298095448E-3</v>
       </c>
       <c r="D7" s="11">
-        <f>AVERAGE('BHNVFEAL data'!AA13:AJ13)*'Calibration Adjustments'!D24</f>
+        <f>AVERAGE('BHNVFEAL data'!AA14:AJ14)*'Calibration Adjustments'!D24</f>
         <v>1.5431879298095448E-3</v>
       </c>
       <c r="E7" s="11">
@@ -11417,7 +11633,7 @@
         <v>3.3970439560149579E-3</v>
       </c>
       <c r="G7" s="18">
-        <f>AVERAGE('BHNVFEAL data'!AA13:AJ13)*'Calibration Adjustments'!G24</f>
+        <f>AVERAGE('BHNVFEAL data'!AA14:AJ14)*'Calibration Adjustments'!G24</f>
         <v>1.5431879298095448E-3</v>
       </c>
       <c r="H7" s="11">
@@ -11441,7 +11657,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:H6"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -11580,8 +11796,8 @@
         <v>17</v>
       </c>
       <c r="B5" s="18">
-        <f>E5*'Calculations Etc'!B3</f>
-        <v>4.8364601990333661E-3</v>
+        <f>AVERAGE('BHNVFEAL data'!C10:AJ10)*'Calibration Adjustments'!B31</f>
+        <v>1.3495815062532836E-2</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -11590,19 +11806,19 @@
         <v>0</v>
       </c>
       <c r="E5" s="18">
-        <f>AVERAGE('BHNVFEAL data'!C10:AJ10)*'Calibration Adjustments'!E31</f>
-        <v>7.0214683806076057E-3</v>
+        <f>AVERAGE('BHNVFEAL data'!C11:AJ11)*'Calibration Adjustments'!E31</f>
+        <v>3.7455550122320732E-3</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <f>AVERAGE('BHNVFEAL data'!C10:AJ10)*'Calibration Adjustments'!G31</f>
+        <f>AVERAGE('BHNVFEAL data'!C11:AJ11)*'Calibration Adjustments'!G31</f>
         <v>0</v>
       </c>
       <c r="H5">
-        <f>AVERAGE('BHNVFEAL data'!D10:AK10)*'Calibration Adjustments'!H31</f>
-        <v>7.0214683806076057E-3</v>
+        <f>AVERAGE('BHNVFEAL data'!D11:AK11)*'Calibration Adjustments'!H31</f>
+        <v>3.7455550122320732E-3</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -11619,18 +11835,18 @@
         <v>0</v>
       </c>
       <c r="E6" s="18">
-        <f>AVERAGE('BHNVFEAL data'!D12:AJ12)*'Calibration Adjustments'!E32</f>
+        <f>AVERAGE('BHNVFEAL data'!D13:AJ13)*'Calibration Adjustments'!E32</f>
         <v>4.2883704019336085E-3</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <f>AVERAGE('BHNVFEAL data'!D12:AJ12)*'Calibration Adjustments'!G32</f>
+        <f>AVERAGE('BHNVFEAL data'!D13:AJ13)*'Calibration Adjustments'!G32</f>
         <v>0</v>
       </c>
       <c r="H6">
-        <f>AVERAGE('BHNVFEAL data'!E12:AK12)*'Calibration Adjustments'!H32</f>
+        <f>AVERAGE('BHNVFEAL data'!E13:AK13)*'Calibration Adjustments'!H32</f>
         <v>4.3483163881942446E-3</v>
       </c>
     </row>
@@ -11647,7 +11863,7 @@
         <v>1.1883392852619099E-3</v>
       </c>
       <c r="D7" s="11">
-        <f>AVERAGE('BHNVFEAL data'!AA14:AJ14)*'Calibration Adjustments'!D33</f>
+        <f>AVERAGE('BHNVFEAL data'!AA15:AJ15)*'Calibration Adjustments'!D33</f>
         <v>1.1883392852619099E-3</v>
       </c>
       <c r="E7" s="11">

</xml_diff>